<commit_message>
FIM RUN 2020Q3 Second Estimate
</commit_message>
<xml_diff>
--- a/data/raw/haver/national_accounts.xlsx
+++ b/data/raw/haver/national_accounts.xlsx
@@ -29562,7 +29562,7 @@
         <v>21157.6</v>
       </c>
       <c r="C204">
-        <v>18584</v>
+        <v>18583.5</v>
       </c>
       <c r="D204">
         <v>113.86</v>
@@ -29574,7 +29574,7 @@
         <v>12917.3</v>
       </c>
       <c r="G204">
-        <v>111.442</v>
+        <v>111.45</v>
       </c>
       <c r="H204">
         <v>111.334</v>
@@ -29679,7 +29679,7 @@
         <v>3183.5</v>
       </c>
       <c r="AP204">
-        <v>533020</v>
+        <v>533712</v>
       </c>
       <c r="AQ204">
         <v>486072</v>
@@ -29697,7 +29697,7 @@
         <v>1212.3</v>
       </c>
       <c r="AV204">
-        <v>734317</v>
+        <v>731137</v>
       </c>
       <c r="AW204">
         <v>15.6</v>

</xml_diff>